<commit_message>
add supervised evaluation metrics to scores
</commit_message>
<xml_diff>
--- a/notebooks/all_scores.xlsx
+++ b/notebooks/all_scores.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Donat\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jessi\Documents\Studium\WS20_21\text analytics\ita_ws20\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B528926-BC9F-421B-A14B-310CC3395864}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27045" yWindow="7725" windowWidth="27165" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27050" yWindow="7730" windowWidth="27170" windowHeight="16440"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="only_unsupervised" sheetId="1" r:id="rId1"/>
+    <sheet name="all_values" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="49">
   <si>
     <t>birch</t>
   </si>
@@ -109,12 +109,75 @@
   </si>
   <si>
     <t>missing values due to only one cluster</t>
+  </si>
+  <si>
+    <t>LSA</t>
+  </si>
+  <si>
+    <t>Spectral Embedding</t>
+  </si>
+  <si>
+    <t>purity</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> adjusted_rand_score</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> adjusted_mutual_info_score</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> precision</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> recall</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> f1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> accuracy</t>
+  </si>
+  <si>
+    <t>without dimension reduction</t>
+  </si>
+  <si>
+    <t>with stopword removal</t>
+  </si>
+  <si>
+    <t>agglomerative clustering</t>
+  </si>
+  <si>
+    <t>dbscan</t>
+  </si>
+  <si>
+    <t>nur ein cluster</t>
+  </si>
+  <si>
+    <t>gaussian mixture</t>
+  </si>
+  <si>
+    <t>kein attribut label</t>
+  </si>
+  <si>
+    <t>mean_shift</t>
+  </si>
+  <si>
+    <t>optics</t>
+  </si>
+  <si>
+    <t>spectral clustering</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> calinski_harabasz</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> davies_bouldin_score</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -137,21 +200,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -287,35 +344,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -336,6 +391,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -351,16 +410,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -637,50 +722,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.6328125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="38.7265625" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.08984375" style="14" customWidth="1"/>
+    <col min="1" max="1" width="23.6328125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="38.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.08984375" style="8" customWidth="1"/>
     <col min="4" max="4" width="24.7265625" customWidth="1"/>
     <col min="5" max="5" width="22.08984375" customWidth="1"/>
     <col min="6" max="6" width="10.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="23" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:7" s="16" customFormat="1" ht="15" thickBot="1">
+      <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="21"/>
-      <c r="G1" s="22"/>
-    </row>
-    <row r="2" spans="1:7" hidden="1">
-      <c r="A2" s="6" t="s">
+      <c r="F1" s="14"/>
+      <c r="G1" s="15"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="8">
         <v>7.9420674763590396E-3</v>
       </c>
       <c r="D2">
@@ -691,14 +776,12 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" hidden="1">
-      <c r="A3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="10" t="s">
+    <row r="3" spans="1:7">
+      <c r="A3" s="34"/>
+      <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="8">
         <v>7.7299540015926399E-3</v>
       </c>
       <c r="D3">
@@ -709,14 +792,12 @@
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" hidden="1">
-      <c r="A4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="10" t="s">
+    <row r="4" spans="1:7">
+      <c r="A4" s="34"/>
+      <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="8">
         <v>1.2463182548871E-2</v>
       </c>
       <c r="D4">
@@ -727,14 +808,12 @@
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" hidden="1">
-      <c r="A5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="10" t="s">
+    <row r="5" spans="1:7">
+      <c r="A5" s="34"/>
+      <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="8">
         <v>-4.4542018590900201E-3</v>
       </c>
       <c r="D5">
@@ -745,32 +824,30 @@
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" s="3" customFormat="1">
-      <c r="A6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="11" t="s">
+    <row r="6" spans="1:7" s="17" customFormat="1">
+      <c r="A6" s="35"/>
+      <c r="B6" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="31">
         <v>0.34972131831695302</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="17">
         <v>1229.8840818730901</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="17">
         <v>0.82482478938725901</v>
       </c>
-      <c r="G6" s="4"/>
+      <c r="G6" s="32"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="8">
         <v>1.15307709893236E-2</v>
       </c>
       <c r="D7">
@@ -781,11 +858,11 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="25"/>
-      <c r="B8" s="10" t="s">
+      <c r="A8" s="22"/>
+      <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="8">
         <v>1.1667054530591499E-2</v>
       </c>
       <c r="D8">
@@ -796,11 +873,11 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="25"/>
-      <c r="B9" s="10" t="s">
+      <c r="A9" s="22"/>
+      <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="8">
         <v>1.2043073130438699E-2</v>
       </c>
       <c r="D9">
@@ -811,11 +888,11 @@
       </c>
     </row>
     <row r="10" spans="1:7" s="2" customFormat="1">
-      <c r="A10" s="25"/>
-      <c r="B10" s="12" t="s">
+      <c r="A10" s="22"/>
+      <c r="B10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="9">
         <v>1.28000109073753E-2</v>
       </c>
       <c r="D10" s="2">
@@ -825,29 +902,29 @@
         <v>7.2197347808609997</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="5" customFormat="1" ht="14" customHeight="1">
-      <c r="A11" s="26"/>
-      <c r="B11" s="13" t="s">
+    <row r="11" spans="1:7" s="3" customFormat="1">
+      <c r="A11" s="23"/>
+      <c r="B11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="10">
         <v>-7.4069455577694704E-2</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="3">
         <v>163.31290658848101</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="3">
         <v>1.12846242194515</v>
       </c>
     </row>
-    <row r="12" spans="1:7" hidden="1">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:7">
+      <c r="A12" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="8">
         <v>1.09421177725906E-2</v>
       </c>
       <c r="D12">
@@ -858,14 +935,12 @@
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" hidden="1">
-      <c r="A13" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="10" t="s">
+    <row r="13" spans="1:7">
+      <c r="A13" s="36"/>
+      <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="8">
         <v>1.03414465709831E-2</v>
       </c>
       <c r="D13">
@@ -876,14 +951,12 @@
       </c>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" hidden="1">
-      <c r="A14" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="10" t="s">
+    <row r="14" spans="1:7">
+      <c r="A14" s="36"/>
+      <c r="B14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="8">
         <v>1.1837042928991799E-2</v>
       </c>
       <c r="D14">
@@ -894,14 +967,12 @@
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" hidden="1">
-      <c r="A15" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="10" t="s">
+    <row r="15" spans="1:7">
+      <c r="A15" s="36"/>
+      <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="8">
         <v>1.18556013819673E-2</v>
       </c>
       <c r="D15">
@@ -912,31 +983,29 @@
       </c>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" s="3" customFormat="1">
-      <c r="A16" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="11" t="s">
+    <row r="16" spans="1:7" s="17" customFormat="1">
+      <c r="A16" s="38"/>
+      <c r="B16" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="31">
         <v>0.26649813816010998</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="17">
         <v>530.32153717491701</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="17">
         <v>0.86236856826196195</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:7">
+      <c r="A17" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="8">
         <v>1.6537574449598999E-3</v>
       </c>
       <c r="D17">
@@ -946,14 +1015,12 @@
         <v>6.8338845397904304</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1">
-      <c r="A18" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="10" t="s">
+    <row r="18" spans="1:7">
+      <c r="A18" s="36"/>
+      <c r="B18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="8">
         <v>3.5813609143844202E-3</v>
       </c>
       <c r="D18">
@@ -963,14 +1030,12 @@
         <v>6.9909933064839</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1">
-      <c r="A19" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="10" t="s">
+    <row r="19" spans="1:7">
+      <c r="A19" s="36"/>
+      <c r="B19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19" s="8">
         <v>9.3050262973277103E-3</v>
       </c>
       <c r="D19">
@@ -981,14 +1046,12 @@
       </c>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" hidden="1">
-      <c r="A20" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="10" t="s">
+    <row r="20" spans="1:7">
+      <c r="A20" s="36"/>
+      <c r="B20" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="8">
         <v>8.1364901538727597E-3</v>
       </c>
       <c r="D20">
@@ -999,28 +1062,26 @@
       </c>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" s="3" customFormat="1">
-      <c r="A21" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="11" t="s">
+    <row r="21" spans="1:7" s="17" customFormat="1">
+      <c r="A21" s="38"/>
+      <c r="B21" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C21" s="31">
         <v>0.32382127055847498</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="17">
         <v>1007.1023735057601</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="17">
         <v>0.88665159302664398</v>
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C22" s="2">
@@ -1035,8 +1096,8 @@
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="28"/>
-      <c r="B23" s="10" t="s">
+      <c r="A23" s="25"/>
+      <c r="B23" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="2">
@@ -1051,8 +1112,8 @@
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="28"/>
-      <c r="B24" s="10" t="s">
+      <c r="A24" s="25"/>
+      <c r="B24" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="2">
@@ -1066,27 +1127,27 @@
       </c>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:7" s="5" customFormat="1">
-      <c r="A25" s="30"/>
-      <c r="B25" s="13" t="s">
+    <row r="25" spans="1:7" s="3" customFormat="1">
+      <c r="A25" s="26"/>
+      <c r="B25" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="29">
+      <c r="C25" s="17">
         <v>0.19808400000000001</v>
       </c>
-      <c r="D25" s="29">
+      <c r="D25" s="17">
         <v>176.75224600000001</v>
       </c>
-      <c r="E25" s="29">
+      <c r="E25" s="17">
         <v>1.2422219999999999</v>
       </c>
-      <c r="F25" s="29"/>
+      <c r="F25" s="17"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="2">
@@ -1101,8 +1162,8 @@
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="28"/>
-      <c r="B27" s="10" t="s">
+      <c r="A27" s="25"/>
+      <c r="B27" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C27" s="2">
@@ -1117,8 +1178,8 @@
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="28"/>
-      <c r="B28" s="10" t="s">
+      <c r="A28" s="25"/>
+      <c r="B28" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C28" s="2">
@@ -1133,8 +1194,8 @@
       <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="28"/>
-      <c r="B29" s="10" t="s">
+      <c r="A29" s="25"/>
+      <c r="B29" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C29" s="2">
@@ -1148,27 +1209,27 @@
       </c>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:7" s="5" customFormat="1">
-      <c r="A30" s="30"/>
-      <c r="B30" s="13" t="s">
+    <row r="30" spans="1:7" s="3" customFormat="1">
+      <c r="A30" s="26"/>
+      <c r="B30" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="29">
+      <c r="C30" s="17">
         <v>0.49760700000000002</v>
       </c>
-      <c r="D30" s="29">
+      <c r="D30" s="17">
         <v>9909.0290540000005</v>
       </c>
-      <c r="E30" s="29">
+      <c r="E30" s="17">
         <v>0.51976500000000003</v>
       </c>
-      <c r="F30" s="29"/>
+      <c r="F30" s="17"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="2">
@@ -1183,8 +1244,8 @@
       <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="28"/>
-      <c r="B32" s="10" t="s">
+      <c r="A32" s="25"/>
+      <c r="B32" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C32" s="2">
@@ -1199,8 +1260,8 @@
       <c r="F32" s="2"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="28"/>
-      <c r="B33" s="10" t="s">
+      <c r="A33" s="25"/>
+      <c r="B33" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C33" s="2" t="s">
@@ -1209,38 +1270,38 @@
       <c r="D33" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E33" s="31" t="s">
+      <c r="E33" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F33" s="31"/>
-      <c r="G33" s="32" t="s">
+      <c r="F33" s="18"/>
+      <c r="G33" s="19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="5" customFormat="1">
-      <c r="A34" s="30"/>
-      <c r="B34" s="13" t="s">
+    <row r="34" spans="1:7" s="3" customFormat="1">
+      <c r="A34" s="26"/>
+      <c r="B34" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="29" t="s">
+      <c r="C34" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="29" t="s">
+      <c r="D34" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E34" s="29" t="s">
+      <c r="E34" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F34" s="29"/>
-      <c r="G34" s="33" t="s">
+      <c r="F34" s="17"/>
+      <c r="G34" s="20" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C35" s="2" t="s">
@@ -1249,36 +1310,36 @@
       <c r="D35" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E35" s="31" t="s">
+      <c r="E35" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F35" s="31"/>
-      <c r="G35" s="32" t="s">
+      <c r="F35" s="18"/>
+      <c r="G35" s="19" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="28"/>
-      <c r="B36" s="10" t="s">
+      <c r="A36" s="25"/>
+      <c r="B36" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C36" s="31" t="s">
+      <c r="C36" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D36" s="31" t="s">
+      <c r="D36" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E36" s="31" t="s">
+      <c r="E36" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F36" s="31"/>
-      <c r="G36" s="32" t="s">
+      <c r="F36" s="18"/>
+      <c r="G36" s="19" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="28"/>
-      <c r="B37" s="10" t="s">
+      <c r="A37" s="25"/>
+      <c r="B37" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C37" s="2">
@@ -1292,27 +1353,27 @@
       </c>
       <c r="F37" s="2"/>
     </row>
-    <row r="38" spans="1:7" s="5" customFormat="1">
-      <c r="A38" s="30"/>
-      <c r="B38" s="13" t="s">
+    <row r="38" spans="1:7" s="3" customFormat="1">
+      <c r="A38" s="26"/>
+      <c r="B38" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="29">
+      <c r="C38" s="17">
         <v>0.58973100000000001</v>
       </c>
-      <c r="D38" s="29">
+      <c r="D38" s="17">
         <v>2831.114227</v>
       </c>
-      <c r="E38" s="29">
+      <c r="E38" s="17">
         <v>0.56457299999999999</v>
       </c>
-      <c r="F38" s="29"/>
+      <c r="F38" s="17"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="27" t="s">
+      <c r="A39" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C39" s="2">
@@ -1327,8 +1388,8 @@
       <c r="F39" s="2"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="28"/>
-      <c r="B40" s="10" t="s">
+      <c r="A40" s="25"/>
+      <c r="B40" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C40" s="2">
@@ -1343,8 +1404,8 @@
       <c r="F40" s="2"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="28"/>
-      <c r="B41" s="10" t="s">
+      <c r="A41" s="25"/>
+      <c r="B41" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C41" s="2">
@@ -1359,8 +1420,8 @@
       <c r="F41" s="2"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="28"/>
-      <c r="B42" s="10" t="s">
+      <c r="A42" s="25"/>
+      <c r="B42" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C42" s="2">
@@ -1375,11 +1436,11 @@
       <c r="F42" s="2"/>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="28"/>
-      <c r="B43" s="10" t="s">
+      <c r="A43" s="25"/>
+      <c r="B43" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C43" s="14">
+      <c r="C43" s="8">
         <v>-0.19117600000000001</v>
       </c>
       <c r="D43">
@@ -1389,21 +1450,21 @@
         <v>1.7889949999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="5" customFormat="1">
-      <c r="A44" s="30"/>
-      <c r="B44" s="13" t="s">
+    <row r="44" spans="1:7" s="3" customFormat="1">
+      <c r="A44" s="26"/>
+      <c r="B44" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C44" s="29">
+      <c r="C44" s="17">
         <v>0.34642299999999998</v>
       </c>
-      <c r="D44" s="29">
+      <c r="D44" s="17">
         <v>41.642623999999998</v>
       </c>
-      <c r="E44" s="29">
+      <c r="E44" s="17">
         <v>1.5343500000000001</v>
       </c>
-      <c r="F44" s="29"/>
+      <c r="F44" s="17"/>
     </row>
     <row r="45" spans="1:7">
       <c r="C45" s="2"/>
@@ -1435,15 +1496,924 @@
       <c r="F49" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
+    <mergeCell ref="A39:A44"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A21"/>
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="A26:A30"/>
     <mergeCell ref="A31:A34"/>
     <mergeCell ref="A35:A38"/>
-    <mergeCell ref="A39:A44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L33"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="2" width="25.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2">
+        <v>3.7394783114001799E-4</v>
+      </c>
+      <c r="D2">
+        <v>5.3477717983515802</v>
+      </c>
+      <c r="E2">
+        <v>8.0836429605374001</v>
+      </c>
+      <c r="F2">
+        <v>0.71227272727272695</v>
+      </c>
+      <c r="G2">
+        <v>4.23271385381307E-2</v>
+      </c>
+      <c r="H2">
+        <v>6.1738125861639098E-2</v>
+      </c>
+      <c r="I2">
+        <v>0.77179014602604601</v>
+      </c>
+      <c r="J2">
+        <v>5.4545454545454501E-2</v>
+      </c>
+      <c r="K2">
+        <v>3.5599616014870203E-2</v>
+      </c>
+      <c r="L2">
+        <v>5.4545454545454501E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="29"/>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3">
+        <v>0.48930006125652398</v>
+      </c>
+      <c r="D3">
+        <v>15107.2054488456</v>
+      </c>
+      <c r="E3">
+        <v>0.51760382328252197</v>
+      </c>
+      <c r="F3">
+        <v>0.71272727272727199</v>
+      </c>
+      <c r="G3">
+        <v>9.30680140923398E-3</v>
+      </c>
+      <c r="H3">
+        <v>1.8598879493516698E-2</v>
+      </c>
+      <c r="I3">
+        <v>0.77928458095969799</v>
+      </c>
+      <c r="J3">
+        <v>0.02</v>
+      </c>
+      <c r="K3">
+        <v>2.3205209303078699E-2</v>
+      </c>
+      <c r="L3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="29"/>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4">
+        <v>0.27392633566428598</v>
+      </c>
+      <c r="D4">
+        <v>1165.07215929525</v>
+      </c>
+      <c r="E4">
+        <v>0.91450958139961103</v>
+      </c>
+      <c r="F4">
+        <v>0.71363636363636296</v>
+      </c>
+      <c r="G4">
+        <v>9.3444111734507403E-3</v>
+      </c>
+      <c r="H4">
+        <v>2.8581792216919401E-2</v>
+      </c>
+      <c r="I4">
+        <v>0.81190630504030403</v>
+      </c>
+      <c r="J4">
+        <v>2.8636363636363599E-2</v>
+      </c>
+      <c r="K4">
+        <v>3.4028795560278498E-2</v>
+      </c>
+      <c r="L4">
+        <v>2.8636363636363599E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="29"/>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5">
+        <v>6.1695025139570005E-4</v>
+      </c>
+      <c r="D5">
+        <v>5.4983470483124597</v>
+      </c>
+      <c r="E5">
+        <v>7.6647763601130103</v>
+      </c>
+      <c r="F5">
+        <v>0.71681818181818102</v>
+      </c>
+      <c r="G5">
+        <v>8.0708978304481704E-2</v>
+      </c>
+      <c r="H5">
+        <v>6.73018518551355E-2</v>
+      </c>
+      <c r="I5">
+        <v>0.77432190782110799</v>
+      </c>
+      <c r="J5">
+        <v>1.09090909090909E-2</v>
+      </c>
+      <c r="K5">
+        <v>1.1162596356730101E-2</v>
+      </c>
+      <c r="L5">
+        <v>1.09090909090909E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6">
+        <v>2.6974322999506698E-3</v>
+      </c>
+      <c r="D6">
+        <v>4.0823423291560497</v>
+      </c>
+      <c r="E6">
+        <v>6.4310944887818904</v>
+      </c>
+      <c r="F6">
+        <v>0.71363636363636296</v>
+      </c>
+      <c r="G6">
+        <v>1.44673046923836E-2</v>
+      </c>
+      <c r="H6">
+        <v>6.3409055900637099E-2</v>
+      </c>
+      <c r="I6">
+        <v>0.73258644266688699</v>
+      </c>
+      <c r="J6">
+        <v>4.0909090909090904E-3</v>
+      </c>
+      <c r="K6">
+        <v>4.4564391629278799E-3</v>
+      </c>
+      <c r="L6">
+        <v>4.0909090909090904E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="29"/>
+      <c r="B7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7">
+        <v>0.49502931265464101</v>
+      </c>
+      <c r="D7">
+        <v>30203.984955333799</v>
+      </c>
+      <c r="E7">
+        <v>0.45411205329431797</v>
+      </c>
+      <c r="F7">
+        <v>0.71545454545454501</v>
+      </c>
+      <c r="G7">
+        <v>4.87675136819466E-3</v>
+      </c>
+      <c r="H7">
+        <v>1.4555605981885799E-2</v>
+      </c>
+      <c r="I7">
+        <v>0.76267181040937504</v>
+      </c>
+      <c r="J7">
+        <v>8.6363636363636295E-3</v>
+      </c>
+      <c r="K7">
+        <v>1.1534982239543599E-2</v>
+      </c>
+      <c r="L7">
+        <v>8.6363636363636295E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="29"/>
+      <c r="B8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="29"/>
+      <c r="B9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9">
+        <v>4.2482638510785804E-3</v>
+      </c>
+      <c r="D9">
+        <v>4.1571602083724901</v>
+      </c>
+      <c r="E9">
+        <v>6.2879706963383803</v>
+      </c>
+      <c r="F9">
+        <v>0.71772727272727199</v>
+      </c>
+      <c r="G9">
+        <v>2.6789809025042199E-2</v>
+      </c>
+      <c r="H9">
+        <v>7.1872691044071596E-2</v>
+      </c>
+      <c r="I9">
+        <v>0.72067815588391304</v>
+      </c>
+      <c r="J9">
+        <v>5.4545454545454498E-3</v>
+      </c>
+      <c r="K9">
+        <v>3.5201776915686602E-3</v>
+      </c>
+      <c r="L9">
+        <v>5.4545454545454498E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10">
+        <v>-1.65626479894792E-2</v>
+      </c>
+      <c r="D10">
+        <v>1.9979030813827099</v>
+      </c>
+      <c r="E10">
+        <v>1.9417207557845</v>
+      </c>
+      <c r="F10">
+        <v>0.71045454545454501</v>
+      </c>
+      <c r="G10">
+        <v>1.6175182884017099E-3</v>
+      </c>
+      <c r="H10">
+        <v>2.5649366416392598E-3</v>
+      </c>
+      <c r="I10">
+        <v>0.63725932561175402</v>
+      </c>
+      <c r="J10">
+        <v>0.70363636363636295</v>
+      </c>
+      <c r="K10">
+        <v>0.58698155039668098</v>
+      </c>
+      <c r="L10">
+        <v>0.70363636363636295</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="29"/>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="29"/>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="29"/>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13">
+        <v>-1.7228306314261501E-2</v>
+      </c>
+      <c r="D13">
+        <v>1.9918286472189</v>
+      </c>
+      <c r="E13">
+        <v>1.9425542993965099</v>
+      </c>
+      <c r="F13">
+        <v>0.71045454545454501</v>
+      </c>
+      <c r="G13">
+        <v>1.6175182884017099E-3</v>
+      </c>
+      <c r="H13">
+        <v>2.5649366416392598E-3</v>
+      </c>
+      <c r="I13">
+        <v>0.63725932561175402</v>
+      </c>
+      <c r="J13">
+        <v>0.70363636363636295</v>
+      </c>
+      <c r="K13">
+        <v>0.58698155039668098</v>
+      </c>
+      <c r="L13">
+        <v>0.70363636363636295</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="29"/>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="29"/>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="29"/>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18">
+        <v>1.09732082755038E-2</v>
+      </c>
+      <c r="D18">
+        <v>4.3986135142051301</v>
+      </c>
+      <c r="E18">
+        <v>6.5212434286576402</v>
+      </c>
+      <c r="F18">
+        <v>0.71454545454545404</v>
+      </c>
+      <c r="G18">
+        <v>1.16626939139231E-2</v>
+      </c>
+      <c r="H18">
+        <v>6.94044261467332E-2</v>
+      </c>
+      <c r="I18">
+        <v>0.70873860121319199</v>
+      </c>
+      <c r="J18">
+        <v>9.0909090909090898E-4</v>
+      </c>
+      <c r="K18">
+        <v>1.8344155844155801E-4</v>
+      </c>
+      <c r="L18">
+        <v>9.0909090909090898E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="29"/>
+      <c r="B19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19">
+        <v>0.54002767065759205</v>
+      </c>
+      <c r="D19">
+        <v>45405.182533014799</v>
+      </c>
+      <c r="E19">
+        <v>0.48822838366432197</v>
+      </c>
+      <c r="F19">
+        <v>0.71318181818181803</v>
+      </c>
+      <c r="G19">
+        <v>2.8383119043338201E-3</v>
+      </c>
+      <c r="H19">
+        <v>1.34494382493285E-2</v>
+      </c>
+      <c r="I19">
+        <v>0.73427787462546801</v>
+      </c>
+      <c r="J19">
+        <v>7.2727272727272701E-3</v>
+      </c>
+      <c r="K19">
+        <v>7.7275099239046104E-3</v>
+      </c>
+      <c r="L19">
+        <v>7.2727272727272701E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="29"/>
+      <c r="B20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20">
+        <v>0.33063502445238102</v>
+      </c>
+      <c r="D20">
+        <v>1344.5473239192199</v>
+      </c>
+      <c r="E20">
+        <v>0.813033783696687</v>
+      </c>
+      <c r="F20">
+        <v>0.71727272727272695</v>
+      </c>
+      <c r="G20">
+        <v>4.5399227721056703E-3</v>
+      </c>
+      <c r="H20">
+        <v>2.14543411960115E-2</v>
+      </c>
+      <c r="I20">
+        <v>0.73865795169742499</v>
+      </c>
+      <c r="J20">
+        <v>6.81818181818181E-3</v>
+      </c>
+      <c r="K20">
+        <v>1.0086688760558999E-2</v>
+      </c>
+      <c r="L20">
+        <v>6.81818181818181E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="29"/>
+      <c r="B21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21">
+        <v>1.0160254056705001E-2</v>
+      </c>
+      <c r="D21">
+        <v>4.3273998446470499</v>
+      </c>
+      <c r="E21">
+        <v>6.6470553814012696</v>
+      </c>
+      <c r="F21">
+        <v>0.71363636363636296</v>
+      </c>
+      <c r="G21">
+        <v>8.7458016454483797E-3</v>
+      </c>
+      <c r="H21">
+        <v>6.1652083342595101E-2</v>
+      </c>
+      <c r="I21">
+        <v>0.80012729938683003</v>
+      </c>
+      <c r="J21">
+        <v>1.2272727272727201E-2</v>
+      </c>
+      <c r="K21">
+        <v>2.1174019607843101E-2</v>
+      </c>
+      <c r="L21">
+        <v>1.2272727272727201E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="29"/>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="29"/>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="29"/>
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="29"/>
+      <c r="B27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27">
+        <v>0.25094279547356602</v>
+      </c>
+      <c r="D27">
+        <v>29.845446395184201</v>
+      </c>
+      <c r="E27">
+        <v>1.5646810147730701</v>
+      </c>
+      <c r="F27">
+        <v>0.71818181818181803</v>
+      </c>
+      <c r="G27">
+        <v>2.5543988263305903E-4</v>
+      </c>
+      <c r="H27">
+        <v>2.0196513572517702E-3</v>
+      </c>
+      <c r="I27">
+        <v>0.50314427224796299</v>
+      </c>
+      <c r="J27">
+        <v>0.18363636363636299</v>
+      </c>
+      <c r="K27">
+        <v>0.26906869446343101</v>
+      </c>
+      <c r="L27">
+        <v>0.18363636363636299</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="29"/>
+      <c r="B28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28">
+        <v>-0.16781224229819799</v>
+      </c>
+      <c r="D28">
+        <v>10.2437883748304</v>
+      </c>
+      <c r="E28">
+        <v>2.0990364647676398</v>
+      </c>
+      <c r="F28">
+        <v>0.71772727272727199</v>
+      </c>
+      <c r="G28">
+        <v>-4.8097864805093796E-3</v>
+      </c>
+      <c r="H28">
+        <v>7.0312017280170502E-3</v>
+      </c>
+      <c r="I28">
+        <v>0.51717350131752304</v>
+      </c>
+      <c r="J28">
+        <v>0.35318181818181799</v>
+      </c>
+      <c r="K28">
+        <v>0.41377445633514098</v>
+      </c>
+      <c r="L28">
+        <v>0.35318181818181799</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="29"/>
+      <c r="B29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="27">
+        <v>8.8766574866163607E-6</v>
+      </c>
+      <c r="D29">
+        <v>2.56260451373833</v>
+      </c>
+      <c r="E29">
+        <v>2.3649120210918002</v>
+      </c>
+      <c r="F29">
+        <v>0.70863636363636295</v>
+      </c>
+      <c r="G29">
+        <v>-3.3129431838187702E-3</v>
+      </c>
+      <c r="H29">
+        <v>-7.5254343182488297E-4</v>
+      </c>
+      <c r="I29">
+        <v>0.78714972043901399</v>
+      </c>
+      <c r="J29">
+        <v>0.70636363636363597</v>
+      </c>
+      <c r="K29">
+        <v>0.58669201336755905</v>
+      </c>
+      <c r="L29">
+        <v>0.70636363636363597</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30">
+        <v>8.7513407664498201E-3</v>
+      </c>
+      <c r="D30">
+        <v>6.2707684610053702</v>
+      </c>
+      <c r="E30">
+        <v>7.5043174324508799</v>
+      </c>
+      <c r="F30">
+        <v>0.71272727272727199</v>
+      </c>
+      <c r="G30">
+        <v>2.57529413836214E-2</v>
+      </c>
+      <c r="H30">
+        <v>7.0139198085002102E-2</v>
+      </c>
+      <c r="I30">
+        <v>0.79753421866855501</v>
+      </c>
+      <c r="J30">
+        <v>1.2272727272727201E-2</v>
+      </c>
+      <c r="K30">
+        <v>1.6814372247642199E-2</v>
+      </c>
+      <c r="L30">
+        <v>1.2272727272727201E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="28"/>
+      <c r="B31" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31">
+        <v>0.25524410303172301</v>
+      </c>
+      <c r="D31">
+        <v>1557.84556275004</v>
+      </c>
+      <c r="E31">
+        <v>0.63011879521893199</v>
+      </c>
+      <c r="F31">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="G31">
+        <v>2.1264208223616399E-2</v>
+      </c>
+      <c r="H31">
+        <v>3.3519193270838202E-2</v>
+      </c>
+      <c r="I31">
+        <v>0.73630798901729699</v>
+      </c>
+      <c r="J31">
+        <v>8.1818181818181807E-3</v>
+      </c>
+      <c r="K31">
+        <v>7.5784964555436702E-4</v>
+      </c>
+      <c r="L31">
+        <v>8.1818181818181807E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="28"/>
+      <c r="B32" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32">
+        <v>-9.1386833916004107E-2</v>
+      </c>
+      <c r="D32">
+        <v>137.15840295056799</v>
+      </c>
+      <c r="E32">
+        <v>0.90359675251455895</v>
+      </c>
+      <c r="F32">
+        <v>0.70954545454545404</v>
+      </c>
+      <c r="G32">
+        <v>-6.0806287549848895E-4</v>
+      </c>
+      <c r="H32">
+        <v>2.40475519919836E-2</v>
+      </c>
+      <c r="I32">
+        <v>0.73637224657408795</v>
+      </c>
+      <c r="J32">
+        <v>1.2272727272727201E-2</v>
+      </c>
+      <c r="K32">
+        <v>8.84644224318672E-4</v>
+      </c>
+      <c r="L32">
+        <v>1.2272727272727201E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="28"/>
+      <c r="B33" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33">
+        <v>9.2471701294876592E-3</v>
+      </c>
+      <c r="D33">
+        <v>6.26041795949246</v>
+      </c>
+      <c r="E33">
+        <v>7.3623578645520604</v>
+      </c>
+      <c r="F33">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="G33">
+        <v>2.7885920489303599E-2</v>
+      </c>
+      <c r="H33">
+        <v>6.8050333565960505E-2</v>
+      </c>
+      <c r="I33">
+        <v>0.810248673939443</v>
+      </c>
+      <c r="J33">
+        <v>1.72727272727272E-2</v>
+      </c>
+      <c r="K33">
+        <v>2.43668126292691E-2</v>
+      </c>
+      <c r="L33">
+        <v>1.72727272727272E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A22:A25"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>